<commit_message>
Added Keyword Frequency Analysis, counts every mention of a word in the job description. This helps determine skills employers are looking for
</commit_message>
<xml_diff>
--- a/ResumeSkillTree.xlsx
+++ b/ResumeSkillTree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curti\Desktop\Python_JobScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78628751-17DB-4840-8802-448C16027A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9CADE0-55C9-437F-BBE4-195720AD5FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5790" yWindow="530" windowWidth="11660" windowHeight="6200" activeTab="2" xr2:uid="{5C5413F8-FB06-403D-ABCF-7BFC04883E28}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="530" windowWidth="11660" windowHeight="6200" activeTab="2" xr2:uid="{5C5413F8-FB06-403D-ABCF-7BFC04883E28}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of Qualifications" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Java</t>
   </si>
@@ -152,9 +152,6 @@
     <t xml:space="preserve">Maintain </t>
   </si>
   <si>
-    <t xml:space="preserve">learn </t>
-  </si>
-  <si>
     <t xml:space="preserve">improve </t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Azure</t>
   </si>
   <si>
-    <t xml:space="preserve">knowledge </t>
-  </si>
-  <si>
     <t xml:space="preserve">UX </t>
   </si>
   <si>
@@ -312,6 +306,18 @@
   </si>
   <si>
     <t xml:space="preserve">Computer-technician Co-op, 2015 - 2016, Northern Business Equipment </t>
+  </si>
+  <si>
+    <t>learn , knowledge</t>
+  </si>
+  <si>
+    <t>Frequently worked as a team to solve problems and increase effieciency.</t>
+  </si>
+  <si>
+    <t>Real Time Analytical Skills allowed for fast and safe deliveries in urban traffic.</t>
+  </si>
+  <si>
+    <t>In an emerging industry I was enthuasiastic to seek knowledge and learn fast.</t>
   </si>
 </sst>
 </file>
@@ -371,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -380,6 +386,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,16 +713,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
@@ -731,21 +740,21 @@
         <v>38</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
@@ -754,13 +763,13 @@
         <v>16</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.35">
@@ -768,14 +777,14 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4"/>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>9</v>
@@ -787,10 +796,10 @@
         <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="31.5" x14ac:dyDescent="0.35">
@@ -798,14 +807,14 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="4"/>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>15</v>
@@ -819,11 +828,11 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="4"/>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>17</v>
@@ -834,11 +843,11 @@
     </row>
     <row r="6" spans="1:18" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2"/>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>23</v>
@@ -850,7 +859,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>24</v>
@@ -861,7 +870,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -878,7 +887,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>22</v>
@@ -889,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -897,7 +906,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K11" s="2"/>
       <c r="P11" s="4" t="s">
@@ -906,10 +915,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>31</v>
@@ -921,19 +930,19 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="F14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>37</v>
@@ -988,13 +997,13 @@
     </row>
     <row r="24" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J24" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J25" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K25" s="3"/>
     </row>
@@ -1015,7 +1024,7 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1031,7 +1040,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1046,21 +1055,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -1144,54 +1153,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721D7DFD-5493-4C46-ABC7-EE67B9AB13EA}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.81640625" customWidth="1"/>
     <col min="2" max="2" width="4.453125" style="5" customWidth="1"/>
-    <col min="3" max="5" width="47.26953125" customWidth="1"/>
+    <col min="3" max="5" width="71.81640625" customWidth="1"/>
     <col min="6" max="14" width="28.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
         <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1201,19 +1214,19 @@
       <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>48</v>
+      <c r="A10" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1224,58 +1237,59 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
     </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>